<commit_message>
Moving common API fields to parent class
Common API: 15 fields
FinanceNow: 11 Fields
EverywhereRemit: 11 Fields
PaymentGo: 9 Fields

Slight update to validation to display proper row number and apiField
</commit_message>
<xml_diff>
--- a/testFiles/Invalid Country.xlsx
+++ b/testFiles/Invalid Country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yu Quan\Documents\Java\src\Project\Object-Orientated-Programming-G2Project\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF583A5-86C6-4C4A-B519-71E2A47636F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C13128-E202-4060-ACC7-E7040C41ED48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F975919-C47D-ED4B-A3EE-295A5CBC72C6}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="151">
   <si>
     <t>First Name</t>
   </si>
@@ -622,19 +622,10 @@
     <t>OOP</t>
   </si>
   <si>
-    <t>OEL</t>
-  </si>
-  <si>
-    <t>XXX</t>
-  </si>
-  <si>
-    <t>ZZZ</t>
-  </si>
-  <si>
-    <t>HIHI</t>
-  </si>
-  <si>
     <t>LOL</t>
+  </si>
+  <si>
+    <t>WOW</t>
   </si>
 </sst>
 </file>
@@ -932,7 +923,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
@@ -985,6 +976,26 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1373,36 +1384,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="31" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="33" t="s">
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="33"/>
+      <c r="X1" s="43"/>
     </row>
     <row r="2" spans="1:24" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -1491,14 +1502,14 @@
       <c r="D3" s="23">
         <v>2</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>55</v>
@@ -1572,7 +1583,7 @@
         <v>54</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>149</v>
+        <v>54</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>55</v>
@@ -1720,7 +1731,7 @@
         <v>54</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>55</v>
@@ -1774,77 +1785,77 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
-      <c r="A7" t="s">
+    <row r="7" spans="1:24" s="29" customFormat="1">
+      <c r="A7" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="30">
         <v>2</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="31">
         <v>31921</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="H7" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="29">
         <v>99</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="29">
         <v>99</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="29">
         <v>23</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="M7" s="29">
+        <v>1</v>
+      </c>
+      <c r="N7" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="29">
         <v>2</v>
       </c>
-      <c r="R7" s="21">
+      <c r="R7" s="31">
         <v>22907</v>
       </c>
-      <c r="S7" s="25" t="s">
+      <c r="S7" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="T7" s="16" t="s">
+      <c r="T7" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="24" t="s">
+      <c r="V7" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="W7" s="22" t="s">
+      <c r="W7" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="X7" s="23">
+      <c r="X7" s="37">
         <v>5000</v>
       </c>
     </row>
@@ -1868,7 +1879,7 @@
         <v>54</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>151</v>
+        <v>54</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>55</v>
@@ -1996,152 +2007,152 @@
         <v>8888</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
-      <c r="A10" t="s">
+    <row r="10" spans="1:24" s="29" customFormat="1">
+      <c r="A10" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="30">
         <v>2</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="31">
         <v>26018</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="H10" s="16" t="s">
+      <c r="G10" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="29">
         <v>99</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="29">
         <v>99</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="29">
         <v>23</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="M10" s="29">
+        <v>1</v>
+      </c>
+      <c r="N10" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="26" t="s">
+      <c r="P10" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="29">
         <v>2</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="31">
         <v>33435</v>
       </c>
-      <c r="S10" s="25" t="s">
+      <c r="S10" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="T10" s="16" t="s">
+      <c r="T10" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="V10" s="24" t="s">
+      <c r="V10" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="W10" s="22" t="s">
+      <c r="W10" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="37">
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
-      <c r="A11" t="s">
+    <row r="11" spans="1:24" s="29" customFormat="1">
+      <c r="A11" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="30">
         <v>2</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="31">
         <v>32906</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="29">
         <v>99</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="29">
         <v>99</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="29">
         <v>23</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="M11" s="29">
+        <v>1</v>
+      </c>
+      <c r="N11" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="P11" s="26" t="s">
+      <c r="P11" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="29">
         <v>2</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="31">
         <v>33819</v>
       </c>
-      <c r="S11" s="25" t="s">
+      <c r="S11" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="T11" s="16" t="s">
+      <c r="T11" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="V11" s="24" t="s">
+      <c r="V11" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="W11" s="22" t="s">
+      <c r="W11" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="X11" s="23">
-        <v>1000</v>
+      <c r="X11" s="37">
+        <v>5555</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -2164,7 +2175,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>153</v>
+        <v>54</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>55</v>
@@ -2618,7 +2629,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="17.399999999999999">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2647,7 +2658,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="17.399999999999999">
-      <c r="A3" s="35"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2674,7 +2685,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="17.399999999999999">
-      <c r="A4" s="35"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2698,7 +2709,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="62.4">
-      <c r="A5" s="35"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
@@ -2722,7 +2733,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="17.399999999999999">
-      <c r="A6" s="35"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
@@ -2746,7 +2757,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="17.399999999999999">
-      <c r="A7" s="35"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2773,7 +2784,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="17.399999999999999">
-      <c r="A8" s="35"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
@@ -2800,7 +2811,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="17.399999999999999">
-      <c r="A9" s="35"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
@@ -2824,7 +2835,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="17.399999999999999">
-      <c r="A10" s="35"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2849,7 +2860,7 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" ht="234">
-      <c r="A11" s="35"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2873,7 +2884,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="124.8">
-      <c r="A12" s="35"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
@@ -2897,7 +2908,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="171.6">
-      <c r="A13" s="35"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
@@ -2921,7 +2932,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="124.8">
-      <c r="A14" s="35"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2945,7 +2956,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="17.399999999999999">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2974,7 +2985,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="17.399999999999999">
-      <c r="A16" s="36"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="7" t="s">
         <v>1</v>
       </c>
@@ -3001,7 +3012,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.399999999999999">
-      <c r="A17" s="36"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="7" t="s">
         <v>2</v>
       </c>
@@ -3025,7 +3036,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="62.4">
-      <c r="A18" s="36"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="7" t="s">
         <v>3</v>
       </c>
@@ -3049,7 +3060,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.399999999999999">
-      <c r="A19" s="36"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -3073,7 +3084,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.399999999999999">
-      <c r="A20" s="36"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="7" t="s">
         <v>6</v>
       </c>
@@ -3097,7 +3108,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.399999999999999">
-      <c r="A21" s="36"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="7" t="s">
         <v>4</v>
       </c>
@@ -3124,7 +3135,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="17.399999999999999">
-      <c r="A22" s="36"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
@@ -3148,7 +3159,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.399999999999999">
-      <c r="A23" s="36"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
@@ -3172,7 +3183,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="16.95" customHeight="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="47" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3198,7 +3209,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="16.95" customHeight="1">
-      <c r="A25" s="37"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="7" t="s">
         <v>34</v>
       </c>
@@ -3225,7 +3236,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="17.399999999999999">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="48" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -3254,7 +3265,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.399999999999999">
-      <c r="A27" s="38"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="7" t="s">
         <v>42</v>
       </c>

</xml_diff>